<commit_message>
Updated wordlist till set 25
</commit_message>
<xml_diff>
--- a/wordlist.xlsx
+++ b/wordlist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
   <si>
     <t>abate</t>
   </si>
@@ -1219,6 +1219,306 @@
   </si>
   <si>
     <t>outcome; unraveling of the plot of a play or work of literature</t>
+  </si>
+  <si>
+    <t>deride</t>
+  </si>
+  <si>
+    <t>to mock</t>
+  </si>
+  <si>
+    <t>derivative</t>
+  </si>
+  <si>
+    <t>something derived; unoriginal</t>
+  </si>
+  <si>
+    <t>desiccate</t>
+  </si>
+  <si>
+    <t>to dry completely</t>
+  </si>
+  <si>
+    <t>desuetude</t>
+  </si>
+  <si>
+    <t>state of disuse</t>
+  </si>
+  <si>
+    <t>desultory</t>
+  </si>
+  <si>
+    <t>random; disconnected; rambling</t>
+  </si>
+  <si>
+    <t>deterrent</t>
+  </si>
+  <si>
+    <t>something that discourages or hinders</t>
+  </si>
+  <si>
+    <t>detraction</t>
+  </si>
+  <si>
+    <t>the act of taking away; derogatory comment on a person’s character</t>
+  </si>
+  <si>
+    <t>diaphanous</t>
+  </si>
+  <si>
+    <t>transparent; fine-textured; insubstantial; vague</t>
+  </si>
+  <si>
+    <t>diatribe</t>
+  </si>
+  <si>
+    <t>bitter verbal attack</t>
+  </si>
+  <si>
+    <t>dichotomy</t>
+  </si>
+  <si>
+    <t>division into two usually contradictory parts</t>
+  </si>
+  <si>
+    <t>diffidence</t>
+  </si>
+  <si>
+    <t>shyness; lack of confidence</t>
+  </si>
+  <si>
+    <t>diffuse</t>
+  </si>
+  <si>
+    <t>to spread out</t>
+  </si>
+  <si>
+    <t>digression</t>
+  </si>
+  <si>
+    <t>act of straying from the main point</t>
+  </si>
+  <si>
+    <t>dirge</t>
+  </si>
+  <si>
+    <t>funeral hymn</t>
+  </si>
+  <si>
+    <t>disabuse</t>
+  </si>
+  <si>
+    <t>to free from a misconception</t>
+  </si>
+  <si>
+    <t>discerning</t>
+  </si>
+  <si>
+    <t>perceptive; exhibiting keen insight and good judgment</t>
+  </si>
+  <si>
+    <t>discomfit</t>
+  </si>
+  <si>
+    <t>to make uneasy; disconcert</t>
+  </si>
+  <si>
+    <t>discordant</t>
+  </si>
+  <si>
+    <t>not in tune</t>
+  </si>
+  <si>
+    <t>discredit</t>
+  </si>
+  <si>
+    <t>to dishonor; disgrace; cause to be doubted</t>
+  </si>
+  <si>
+    <t>discrepancy</t>
+  </si>
+  <si>
+    <t>difference between</t>
+  </si>
+  <si>
+    <t>discrete</t>
+  </si>
+  <si>
+    <t>constituting a separate thing; distinct</t>
+  </si>
+  <si>
+    <t>discretion</t>
+  </si>
+  <si>
+    <t>quality of showing self-restraint in speech or actions; circumspection; freedom to act on one’s own</t>
+  </si>
+  <si>
+    <t>disingenuous</t>
+  </si>
+  <si>
+    <t>not candid; crafty</t>
+  </si>
+  <si>
+    <t>disinterested</t>
+  </si>
+  <si>
+    <t>unprejudiced; objective</t>
+  </si>
+  <si>
+    <t>disjointed</t>
+  </si>
+  <si>
+    <t>lacking order or coherence; dislocated</t>
+  </si>
+  <si>
+    <t>dismiss</t>
+  </si>
+  <si>
+    <t>put away from consideration; reject</t>
+  </si>
+  <si>
+    <t>disparage</t>
+  </si>
+  <si>
+    <t>to belittle</t>
+  </si>
+  <si>
+    <t>disparate</t>
+  </si>
+  <si>
+    <t>dissimilar</t>
+  </si>
+  <si>
+    <t>dissemble</t>
+  </si>
+  <si>
+    <t>to pretend; disguise one’s motives</t>
+  </si>
+  <si>
+    <t>disseminate</t>
+  </si>
+  <si>
+    <t>to spread; scatter; disperse</t>
+  </si>
+  <si>
+    <t>dissident</t>
+  </si>
+  <si>
+    <t>person who disagrees about beliefs, etc.</t>
+  </si>
+  <si>
+    <t>dissolution</t>
+  </si>
+  <si>
+    <t>disintegration; debauchery</t>
+  </si>
+  <si>
+    <t>dissonance</t>
+  </si>
+  <si>
+    <t>discord; lack of harmony</t>
+  </si>
+  <si>
+    <t>distend</t>
+  </si>
+  <si>
+    <t>to expand; swell out</t>
+  </si>
+  <si>
+    <t>distill</t>
+  </si>
+  <si>
+    <t>extract the essential elements</t>
+  </si>
+  <si>
+    <t>distrait</t>
+  </si>
+  <si>
+    <t>inattentive; preoccupied</t>
+  </si>
+  <si>
+    <t>diverge</t>
+  </si>
+  <si>
+    <t>to vary; go in different directions from the same point</t>
+  </si>
+  <si>
+    <t>divest</t>
+  </si>
+  <si>
+    <t>to strip; deprive; rid</t>
+  </si>
+  <si>
+    <t>divulge</t>
+  </si>
+  <si>
+    <t>to make known something that is secret</t>
+  </si>
+  <si>
+    <t>doctrinaire</t>
+  </si>
+  <si>
+    <t>relating to a person who cannot compromise about points of a theory or doctrine; dogmatic; unyielding</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>to provide with written evidence to support</t>
+  </si>
+  <si>
+    <t>doggerel</t>
+  </si>
+  <si>
+    <t>poor verse</t>
+  </si>
+  <si>
+    <t>dogmatic</t>
+  </si>
+  <si>
+    <t>stating opinions without proof</t>
+  </si>
+  <si>
+    <t>dormant</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>dross</t>
+  </si>
+  <si>
+    <t>waste; worthless matter; trivial matter</t>
+  </si>
+  <si>
+    <t>dupe</t>
+  </si>
+  <si>
+    <t>to deceive; trick</t>
+  </si>
+  <si>
+    <t>ebullient</t>
+  </si>
+  <si>
+    <t>exhilarated; enthusiastic</t>
+  </si>
+  <si>
+    <t>eclectic</t>
+  </si>
+  <si>
+    <t>selecting from various sources</t>
+  </si>
+  <si>
+    <t>effervescence</t>
+  </si>
+  <si>
+    <t>state of high spirits or liveliness; the process of bubbling as gas escapes</t>
+  </si>
+  <si>
+    <t>effete</t>
+  </si>
+  <si>
+    <t>depleted of vitality; overrefined; decadent</t>
   </si>
 </sst>
 </file>
@@ -1344,15 +1644,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1657,11 +1951,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B233"/>
+  <dimension ref="A1:B288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="B228" sqref="B228"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1669,1710 +1961,2156 @@
     <col min="2" max="2" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="7" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="15"/>
-      <c r="B73" s="15"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="5" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="15"/>
-      <c r="B84" s="15"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="10" t="s">
+      <c r="A87" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+      <c r="A91" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+      <c r="A93" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B94" s="7" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
-      <c r="B95" s="15"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="15"/>
-      <c r="B96" s="15"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
     </row>
     <row r="97" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="15"/>
-      <c r="B97" s="15"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="3" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="5" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
+      <c r="A101" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="5" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
+      <c r="A103" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
+      <c r="A104" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B105" s="11" t="s">
+      <c r="B105" s="5" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
+      <c r="A106" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B106" s="5" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="7" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="15"/>
-      <c r="B108" s="15"/>
+      <c r="A108" s="9"/>
+      <c r="B108" s="9"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+      <c r="A109" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="s">
+      <c r="A110" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="5" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
+      <c r="A111" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="5" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B112" s="5" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B113" s="11" t="s">
+      <c r="B113" s="5" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="10" t="s">
+      <c r="A114" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="5" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="10" t="s">
+      <c r="A115" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B115" s="11" t="s">
+      <c r="B115" s="5" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="10" t="s">
+      <c r="A116" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="10" t="s">
+      <c r="A117" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="B117" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="12" t="s">
+      <c r="A118" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B118" s="13" t="s">
+      <c r="B118" s="7" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="15"/>
-      <c r="B119" s="15"/>
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
+      <c r="A120" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="5" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="10" t="s">
+      <c r="A122" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B122" s="11" t="s">
+      <c r="B122" s="5" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="10" t="s">
+      <c r="A123" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="5" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="10" t="s">
+      <c r="A124" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="5" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="10" t="s">
+      <c r="A125" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="B125" s="5" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="10" t="s">
+      <c r="A126" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B126" s="11" t="s">
+      <c r="B126" s="5" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B127" s="11" t="s">
+      <c r="B127" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="10" t="s">
+      <c r="A128" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B128" s="11" t="s">
+      <c r="B128" s="5" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="15"/>
-      <c r="B130" s="15"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="8" t="s">
+      <c r="A131" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B131" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="10" t="s">
+      <c r="A132" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B132" s="11" t="s">
+      <c r="B132" s="5" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="10" t="s">
+      <c r="A133" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B133" s="11" t="s">
+      <c r="B133" s="5" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="10" t="s">
+      <c r="A134" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B134" s="11" t="s">
+      <c r="B134" s="5" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="10" t="s">
+      <c r="A135" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B135" s="11" t="s">
+      <c r="B135" s="5" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="10" t="s">
+      <c r="A136" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B136" s="11" t="s">
+      <c r="B136" s="5" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="10" t="s">
+      <c r="A137" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B137" s="11" t="s">
+      <c r="B137" s="5" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="10" t="s">
+      <c r="A138" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B138" s="11" t="s">
+      <c r="B138" s="5" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="10" t="s">
+      <c r="A139" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B139" s="11" t="s">
+      <c r="B139" s="5" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="12" t="s">
+      <c r="A140" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="B140" s="13" t="s">
+      <c r="B140" s="7" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="15"/>
-      <c r="B141" s="15"/>
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="15"/>
-      <c r="B142" s="15"/>
+      <c r="A142" s="9"/>
+      <c r="B142" s="9"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="15"/>
-      <c r="B143" s="15"/>
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="15"/>
-      <c r="B144" s="15"/>
+      <c r="A144" s="9"/>
+      <c r="B144" s="9"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="15"/>
-      <c r="B145" s="15"/>
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
     </row>
     <row r="146" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="15"/>
-      <c r="B146" s="15"/>
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="8" t="s">
+      <c r="A147" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B147" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="10" t="s">
+      <c r="A148" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B148" s="11" t="s">
+      <c r="B148" s="5" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="10" t="s">
+      <c r="A149" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B149" s="11" t="s">
+      <c r="B149" s="5" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="10" t="s">
+      <c r="A150" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="5" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="10" t="s">
+      <c r="A151" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B151" s="11" t="s">
+      <c r="B151" s="5" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="10" t="s">
+      <c r="A152" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B152" s="11" t="s">
+      <c r="B152" s="5" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="10" t="s">
+      <c r="A153" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B153" s="11" t="s">
+      <c r="B153" s="5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="10" t="s">
+      <c r="A154" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="5" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="10" t="s">
+      <c r="A155" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B155" s="11" t="s">
+      <c r="B155" s="5" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="12" t="s">
+      <c r="A156" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B156" s="13" t="s">
+      <c r="B156" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="15"/>
-      <c r="B157" s="15"/>
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="8" t="s">
+      <c r="A158" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B158" s="9" t="s">
+      <c r="B158" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="10" t="s">
+      <c r="A159" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B159" s="11" t="s">
+      <c r="B159" s="5" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A160" s="10" t="s">
+      <c r="A160" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B160" s="11" t="s">
+      <c r="B160" s="5" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="10" t="s">
+      <c r="A161" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B161" s="11" t="s">
+      <c r="B161" s="5" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="10" t="s">
+      <c r="A162" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B162" s="11" t="s">
+      <c r="B162" s="5" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="10" t="s">
+      <c r="A163" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B163" s="11" t="s">
+      <c r="B163" s="5" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="10" t="s">
+      <c r="A164" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B164" s="11" t="s">
+      <c r="B164" s="5" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="10" t="s">
+      <c r="A165" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B165" s="11" t="s">
+      <c r="B165" s="5" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="10" t="s">
+      <c r="A166" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B166" s="11" t="s">
+      <c r="B166" s="5" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="12" t="s">
+      <c r="A167" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B167" s="13" t="s">
+      <c r="B167" s="7" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="15"/>
-      <c r="B168" s="15"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="9"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="8" t="s">
+      <c r="A169" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B169" s="9" t="s">
+      <c r="B169" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="10" t="s">
+      <c r="A170" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B170" s="11" t="s">
+      <c r="B170" s="5" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="10" t="s">
+      <c r="A171" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B171" s="11" t="s">
+      <c r="B171" s="5" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="10" t="s">
+      <c r="A172" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B172" s="11" t="s">
+      <c r="B172" s="5" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="10" t="s">
+      <c r="A173" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B173" s="11" t="s">
+      <c r="B173" s="5" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="10" t="s">
+      <c r="A174" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B174" s="11" t="s">
+      <c r="B174" s="5" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="10" t="s">
+      <c r="A175" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="B175" s="11" t="s">
+      <c r="B175" s="5" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="10" t="s">
+      <c r="A176" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B176" s="11" t="s">
+      <c r="B176" s="5" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="10" t="s">
+      <c r="A177" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B177" s="11" t="s">
+      <c r="B177" s="5" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="12" t="s">
+      <c r="A178" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B178" s="13" t="s">
+      <c r="B178" s="7" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="9"/>
+      <c r="B179" s="9"/>
+    </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B180" s="7" t="s">
+      <c r="B180" s="3" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="5" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B182" s="5" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B183" s="5" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="5" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B185" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B186" s="5" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="s">
+      <c r="A187" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="5" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="3" t="s">
+      <c r="A188" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B188" s="5" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="5" t="s">
+      <c r="A189" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="B189" s="7" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+    <row r="190" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="9"/>
+      <c r="B190" s="9"/>
+    </row>
+    <row r="191" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="3" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="A192" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="5" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="A193" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="5" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="A194" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="5" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="A195" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="5" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="A196" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="5" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="A197" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="5" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="A198" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="5" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="A199" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="5" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="200" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="7" t="s">
         <v>339</v>
       </c>
     </row>
+    <row r="201" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="9"/>
+      <c r="B201" s="9"/>
+    </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="A202" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="3" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="A203" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="5" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="A204" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="5" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="A205" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="5" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="A206" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="5" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="A207" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="5" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="A208" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="5" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="A209" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="5" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="210" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="5" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="211" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="7" t="s">
         <v>359</v>
       </c>
     </row>
+    <row r="212" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="9"/>
+      <c r="B212" s="9"/>
+    </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="A213" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="3" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="A214" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="5" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="A215" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="5" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="A216" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="5" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="A217" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="5" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="A218" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="5" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="A219" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="5" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="A220" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B220" s="5" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="A221" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B221" s="5" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="222" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="7" t="s">
         <v>379</v>
       </c>
     </row>
+    <row r="223" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="9"/>
+      <c r="B223" s="9"/>
+    </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+      <c r="A224" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B224" s="3" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+      <c r="A225" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B225" s="5" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
+      <c r="A226" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B226" s="5" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+      <c r="A227" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B227" s="5" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+      <c r="A228" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B228" s="5" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
+      <c r="A229" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B229" s="5" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
+      <c r="A230" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B230" s="5" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
+      <c r="A231" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B231" s="5" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
+      <c r="A232" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B232" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+    <row r="233" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B233" s="7" t="s">
         <v>399</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="9"/>
+      <c r="B234" s="9"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B243" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B244" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="9"/>
+      <c r="B245" s="9"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B255" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="9"/>
+      <c r="B256" s="9"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A258" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B266" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="9"/>
+      <c r="B267" s="9"/>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B269" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B270" s="5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B271" s="5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A277" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="B277" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A278" s="9"/>
+      <c r="B278" s="9"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B285" s="5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="B288" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>